<commit_message>
Update to mail merge population that orders the cards so that they will be in order after stacking the four card groups after cuts
</commit_message>
<xml_diff>
--- a/utils/Mail Merge Data Template.xlsx
+++ b/utils/Mail Merge Data Template.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kurtm\Documents\Repositories\LUMEX\Machita\checkins-datasheet\utils\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE2E9486-9134-4A10-9462-480E4CA8F4D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AB18B47-4DEA-4C9B-978F-C76E678F4B7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{A1651018-6D4C-419B-82B3-24BD91057B40}"/>
+    <workbookView xWindow="28680" yWindow="-60" windowWidth="29040" windowHeight="15840" xr2:uid="{A1651018-6D4C-419B-82B3-24BD91057B40}"/>
   </bookViews>
   <sheets>
     <sheet name="CheckinData" sheetId="9" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">CheckinData!$A$1:$P$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">CheckinData!$A$1:$Q$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Teacher</t>
   </si>
@@ -94,7 +94,10 @@
     <t>Value 5</t>
   </si>
   <si>
-    <t>ClassName</t>
+    <t>Card #</t>
+  </si>
+  <si>
+    <t>Page</t>
   </si>
 </sst>
 </file>
@@ -472,46 +475,48 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3739B2CB-66FD-4290-B7F9-DF1E5B177053}">
-  <dimension ref="A1:P2"/>
+  <dimension ref="A1:Q2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="8" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="81.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="8" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="81.140625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="8" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="19" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="22.109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="22.140625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="18" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="23.88671875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="15.5546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="17" max="28" width="12.44140625" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="8.109375" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="19" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="22.109375" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="18" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="36.6640625" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="15.5546875" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="37" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="12.44140625" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="20" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="8.88671875" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="21.6640625" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="20" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="16.109375" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="33.33203125" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="27" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="19" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="18" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="36.7109375" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="37" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="20" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="20" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="33.28515625" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="14.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -560,10 +565,13 @@
       <c r="P1" t="s">
         <v>15</v>
       </c>
+      <c r="Q1" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="2" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <autoFilter ref="A1:P1" xr:uid="{3739B2CB-66FD-4290-B7F9-DF1E5B177053}"/>
+  <autoFilter ref="A1:Q1" xr:uid="{3739B2CB-66FD-4290-B7F9-DF1E5B177053}"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>